<commit_message>
Cleaned up the code, tested on another machine and added one extra model - super large sentence encoder :)
</commit_message>
<xml_diff>
--- a/classified_requirements.xlsx
+++ b/classified_requirements.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.2061612910514417</v>
+        <v>0.6077384310987872</v>
       </c>
     </row>
     <row r="3">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.2025979481521361</v>
+        <v>0.5676121371873883</v>
       </c>
     </row>
     <row r="4">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.2034154109805173</v>
+        <v>0.5807473489652029</v>
       </c>
     </row>
     <row r="5">
@@ -548,7 +548,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.192586022615491</v>
+        <v>0.577983822890715</v>
       </c>
     </row>
     <row r="6">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.2267699161353894</v>
+        <v>0.6875973831561824</v>
       </c>
     </row>
     <row r="7">
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.2482401013255854</v>
+        <v>0.6585521373376819</v>
       </c>
     </row>
     <row r="8">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.2464001466747738</v>
+        <v>0.6745876697238239</v>
       </c>
     </row>
     <row r="9">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.2491538574872023</v>
+        <v>0.7029086160885609</v>
       </c>
     </row>
     <row r="10">
@@ -673,7 +673,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.1983692440023894</v>
+        <v>0.5690872017843593</v>
       </c>
     </row>
     <row r="11">
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.1931361093379365</v>
+        <v>0.5604340364267851</v>
       </c>
     </row>
     <row r="12">
@@ -723,7 +723,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.202196756181634</v>
+        <v>0.6246528812023089</v>
       </c>
     </row>
     <row r="13">
@@ -748,7 +748,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.2361850624880329</v>
+        <v>0.6566125041370295</v>
       </c>
     </row>
     <row r="14">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.2176903817061423</v>
+        <v>0.5970461390090313</v>
       </c>
     </row>
     <row r="15">
@@ -798,7 +798,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.2312099411263695</v>
+        <v>0.6516624992957248</v>
       </c>
     </row>
     <row r="16">
@@ -823,7 +823,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.2162956432321904</v>
+        <v>0.5863605729765066</v>
       </c>
     </row>
     <row r="17">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.2365807474574455</v>
+        <v>0.6592956398669667</v>
       </c>
     </row>
     <row r="18">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.2048462510828243</v>
+        <v>0.6140413528525036</v>
       </c>
     </row>
     <row r="19">
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.1995071769760643</v>
+        <v>0.5739420476360719</v>
       </c>
     </row>
     <row r="20">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.1909307765708602</v>
+        <v>0.5608710684452218</v>
       </c>
     </row>
     <row r="21">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.1791252463470673</v>
+        <v>0.5436471462903746</v>
       </c>
     </row>
     <row r="22">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.1841692006041259</v>
+        <v>0.5348007727792031</v>
       </c>
     </row>
     <row r="23">
@@ -998,7 +998,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.2031039634145646</v>
+        <v>0.7002801311176623</v>
       </c>
     </row>
     <row r="24">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.2411696302365539</v>
+        <v>0.6785881524847925</v>
       </c>
     </row>
     <row r="25">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.1832100674816395</v>
+        <v>0.5647252059872219</v>
       </c>
     </row>
     <row r="26">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.2390467767806703</v>
+        <v>0.6680321697468004</v>
       </c>
     </row>
     <row r="27">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.212796106016991</v>
+        <v>0.5968168985724113</v>
       </c>
     </row>
     <row r="28">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.244199360467337</v>
+        <v>0.6875826968663854</v>
       </c>
     </row>
     <row r="29">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.1977569631857116</v>
+        <v>0.5718188593859584</v>
       </c>
     </row>
     <row r="30">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0.207058493848454</v>
+        <v>0.5765003501019581</v>
       </c>
     </row>
     <row r="31">
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.2426789978175963</v>
+        <v>0.6655729117738267</v>
       </c>
     </row>
     <row r="32">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.2065915182067066</v>
+        <v>0.6440185094176631</v>
       </c>
     </row>
     <row r="33">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.2123564226936483</v>
+        <v>0.6110080358820285</v>
       </c>
     </row>
     <row r="34">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.2318554821407856</v>
+        <v>0.6815444062738008</v>
       </c>
     </row>
     <row r="35">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,7 +1307,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.2201242573856594</v>
+        <v>0.6834763353675209</v>
       </c>
     </row>
     <row r="36">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.1958988276637397</v>
+        <v>0.5641521724472557</v>
       </c>
     </row>
     <row r="37">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.1990634084442686</v>
+        <v>0.666780003879725</v>
       </c>
     </row>
     <row r="38">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.1814454871708435</v>
+        <v>0.5535057892274129</v>
       </c>
     </row>
     <row r="39">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.2329480353553873</v>
+        <v>0.6518979155981524</v>
       </c>
     </row>
     <row r="40">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.233798156357161</v>
+        <v>0.6356216615246701</v>
       </c>
     </row>
     <row r="41">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0.2116545766132362</v>
+        <v>0.6256987787171775</v>
       </c>
     </row>
     <row r="42">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.2436634483316407</v>
+        <v>0.6920849156503396</v>
       </c>
     </row>
     <row r="43">
@@ -1507,7 +1507,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.2408071375224229</v>
+        <v>0.6846679969513726</v>
       </c>
     </row>
     <row r="44">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.1894993171609753</v>
+        <v>0.5552099764744204</v>
       </c>
     </row>
     <row r="45">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.2184211632593074</v>
+        <v>0.6867315462096182</v>
       </c>
     </row>
     <row r="46">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.209178268968018</v>
+        <v>0.6226865745606156</v>
       </c>
     </row>
     <row r="47">
@@ -1607,7 +1607,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.2466007910943694</v>
+        <v>0.6918521239613371</v>
       </c>
     </row>
     <row r="48">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.1989118940464753</v>
+        <v>0.6240995449824275</v>
       </c>
     </row>
     <row r="49">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.227176951264811</v>
+        <v>0.6986081537989165</v>
       </c>
     </row>
     <row r="50">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.1817814854527411</v>
+        <v>0.5410678101919424</v>
       </c>
     </row>
     <row r="51">
@@ -1707,7 +1707,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.2470349421394815</v>
+        <v>0.6949363903702647</v>
       </c>
     </row>
     <row r="52">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>0.2441060548402795</v>
+        <v>0.6659942091969222</v>
       </c>
     </row>
     <row r="53">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0.209006576308492</v>
+        <v>0.587471636619973</v>
       </c>
     </row>
     <row r="54">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0.1930981390024901</v>
+        <v>0.5691297066792967</v>
       </c>
     </row>
     <row r="55">
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>0.1944617698026087</v>
+        <v>0.5614261326668378</v>
       </c>
     </row>
     <row r="56">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>0.2439058332190712</v>
+        <v>0.6877941059193086</v>
       </c>
     </row>
     <row r="57">
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>0.2194328837598004</v>
+        <v>0.7256233846173087</v>
       </c>
     </row>
     <row r="58">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>0.2451619946144038</v>
+        <v>0.6974494397345261</v>
       </c>
     </row>
     <row r="59">
@@ -1907,7 +1907,7 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>0.2465880402747253</v>
+        <v>0.6619611095095291</v>
       </c>
     </row>
     <row r="60">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>0.2240872039180002</v>
+        <v>0.6624516462878558</v>
       </c>
     </row>
     <row r="61">
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>0.2465318222807898</v>
+        <v>0.6785698847089061</v>
       </c>
     </row>
     <row r="62">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0.205471809075969</v>
+        <v>0.5721511379575926</v>
       </c>
     </row>
     <row r="63">
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0.2414006404411606</v>
+        <v>0.6669702385544822</v>
       </c>
     </row>
     <row r="64">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.2003240792533399</v>
+        <v>0.567710888433699</v>
       </c>
     </row>
     <row r="65">
@@ -2057,7 +2057,7 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.1749353005801892</v>
+        <v>0.5241378914469227</v>
       </c>
     </row>
     <row r="66">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>0.2106803632036459</v>
+        <v>0.6309033577831158</v>
       </c>
     </row>
     <row r="67">
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>0.181737101803323</v>
+        <v>0.5270145400899887</v>
       </c>
     </row>
     <row r="68">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0.2031616044390916</v>
+        <v>0.5734978827351047</v>
       </c>
     </row>
     <row r="69">
@@ -2157,7 +2157,7 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0.2411783640033435</v>
+        <v>0.6621156476400103</v>
       </c>
     </row>
     <row r="70">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>0.1951344996135554</v>
+        <v>0.5549423931360536</v>
       </c>
     </row>
     <row r="71">
@@ -2207,7 +2207,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.187487218504061</v>
+        <v>0.5592027956857066</v>
       </c>
     </row>
     <row r="72">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.2149964620431609</v>
+        <v>0.6079451639677238</v>
       </c>
     </row>
     <row r="73">
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0.2014044064938049</v>
+        <v>0.5937733520479671</v>
       </c>
     </row>
     <row r="74">
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.2463448114985736</v>
+        <v>0.6771617282013017</v>
       </c>
     </row>
     <row r="75">
@@ -2307,7 +2307,7 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.2303657394693001</v>
+        <v>0.6424575790978876</v>
       </c>
     </row>
     <row r="76">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2332,7 +2332,7 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.1847941043961451</v>
+        <v>0.5539725274224939</v>
       </c>
     </row>
     <row r="77">
@@ -2357,7 +2357,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.2432506604572154</v>
+        <v>0.6701871539113655</v>
       </c>
     </row>
     <row r="78">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.2137897493747982</v>
+        <v>0.6334426128454733</v>
       </c>
     </row>
     <row r="79">
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.2036271182853243</v>
+        <v>0.5597900734724914</v>
       </c>
     </row>
     <row r="80">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2432,7 +2432,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.2151059803808965</v>
+        <v>0.6310394252531588</v>
       </c>
     </row>
     <row r="81">
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.1959748629306112</v>
+        <v>0.6161758231208476</v>
       </c>
     </row>
     <row r="82">
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.212245094826251</v>
+        <v>0.6146393793606026</v>
       </c>
     </row>
     <row r="83">
@@ -2507,7 +2507,7 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0.216482286941728</v>
+        <v>0.6445522025907785</v>
       </c>
     </row>
     <row r="84">
@@ -2532,7 +2532,7 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.2103437344564799</v>
+        <v>0.6036984693615891</v>
       </c>
     </row>
     <row r="85">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2557,7 +2557,7 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.1901563618027113</v>
+        <v>0.5746635055979473</v>
       </c>
     </row>
     <row r="86">
@@ -2582,7 +2582,7 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.1810163154559154</v>
+        <v>0.5748408061268547</v>
       </c>
     </row>
     <row r="87">
@@ -2607,7 +2607,7 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.2197733864184454</v>
+        <v>0.6566415377713357</v>
       </c>
     </row>
     <row r="88">
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.2424062340639414</v>
+        <v>0.6611246413887588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All requirements in the same file
</commit_message>
<xml_diff>
--- a/classified_requirements.xlsx
+++ b/classified_requirements.xlsx
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.5499301442546708</v>
+        <v>0.1975625369094737</v>
       </c>
     </row>
     <row r="3">
@@ -498,7 +498,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.6077384336453332</v>
+        <v>0.2061613149769995</v>
       </c>
     </row>
     <row r="4">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.5676121332743115</v>
+        <v>0.2025980125461454</v>
       </c>
     </row>
     <row r="5">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.5312290928545537</v>
+        <v>0.1868822830613323</v>
       </c>
     </row>
     <row r="6">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.5807473484346115</v>
+        <v>0.2034153787161905</v>
       </c>
     </row>
     <row r="7">
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.6012755686123338</v>
+        <v>0.2113910742690737</v>
       </c>
     </row>
     <row r="8">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.5708966791217351</v>
+        <v>0.207674616135464</v>
       </c>
     </row>
     <row r="9">
@@ -648,7 +648,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.5463720423430538</v>
+        <v>0.1922865105919108</v>
       </c>
     </row>
     <row r="10">
@@ -673,7 +673,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.6239796828702286</v>
+        <v>0.2571863448253576</v>
       </c>
     </row>
     <row r="11">
@@ -698,7 +698,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.5779838481842212</v>
+        <v>0.1925860832144265</v>
       </c>
     </row>
     <row r="12">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.5829760169119266</v>
+        <v>0.205629497367141</v>
       </c>
     </row>
     <row r="13">
@@ -748,7 +748,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.6010802907490935</v>
+        <v>0.1943608759190325</v>
       </c>
     </row>
     <row r="14">
@@ -773,7 +773,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.6010802907490935</v>
+        <v>0.1943608759190325</v>
       </c>
     </row>
     <row r="15">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.5438571895870087</v>
+        <v>0.1844892307088042</v>
       </c>
     </row>
     <row r="16">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.5985032272790092</v>
+        <v>0.2053560458429807</v>
       </c>
     </row>
     <row r="17">
@@ -848,7 +848,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.6041486712443926</v>
+        <v>0.2141004860485805</v>
       </c>
     </row>
     <row r="18">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.5524975873489711</v>
+        <v>0.2031009668302029</v>
       </c>
     </row>
     <row r="19">
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.5716317419159489</v>
+        <v>0.20326153281383</v>
       </c>
     </row>
     <row r="20">
@@ -923,7 +923,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.9358487851385324</v>
+        <v>0.2912154967317269</v>
       </c>
     </row>
     <row r="21">
@@ -948,7 +948,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.5981729456476114</v>
+        <v>0.2157136964478057</v>
       </c>
     </row>
     <row r="22">
@@ -973,7 +973,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.6984846990274242</v>
+        <v>0.2391499888644296</v>
       </c>
     </row>
     <row r="23">
@@ -998,7 +998,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.6984846990274242</v>
+        <v>0.2391499888644296</v>
       </c>
     </row>
     <row r="24">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.5854657424584891</v>
+        <v>0.2175129197556451</v>
       </c>
     </row>
     <row r="25">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.7072565685412713</v>
+        <v>0.2414600400545619</v>
       </c>
     </row>
     <row r="26">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.7072565685412713</v>
+        <v>0.2414600400545619</v>
       </c>
     </row>
     <row r="27">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.7312841042539824</v>
+        <v>0.2472072109009033</v>
       </c>
     </row>
     <row r="28">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.7312841042539824</v>
+        <v>0.2472072109009033</v>
       </c>
     </row>
     <row r="29">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.6394599987541907</v>
+        <v>0.2208672147192573</v>
       </c>
     </row>
     <row r="30">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0.6312011866426058</v>
+        <v>0.2370852785282545</v>
       </c>
     </row>
     <row r="31">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.6312011866426058</v>
+        <v>0.2370852785282545</v>
       </c>
     </row>
     <row r="32">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.5910636636474245</v>
+        <v>0.1838901702231884</v>
       </c>
     </row>
     <row r="33">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.6875973598435742</v>
+        <v>0.2267699453509219</v>
       </c>
     </row>
     <row r="34">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.9358487851385324</v>
+        <v>0.2912154967317269</v>
       </c>
     </row>
     <row r="35">
@@ -1307,7 +1307,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.6056152751804642</v>
+        <v>0.2313739633376953</v>
       </c>
     </row>
     <row r="36">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.5693088793416946</v>
+        <v>0.1873363661371938</v>
       </c>
     </row>
     <row r="37">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.5693088793416946</v>
+        <v>0.1873363661371938</v>
       </c>
     </row>
     <row r="38">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.6398100285980376</v>
+        <v>0.2450618499561862</v>
       </c>
     </row>
     <row r="39">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.6512444075423149</v>
+        <v>0.2233997900779244</v>
       </c>
     </row>
     <row r="40">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.6377486460892298</v>
+        <v>0.2290913358032343</v>
       </c>
     </row>
     <row r="41">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0.6037490938843546</v>
+        <v>0.2171766644087157</v>
       </c>
     </row>
     <row r="42">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.6721037326271695</v>
+        <v>0.238384853319791</v>
       </c>
     </row>
     <row r="43">
@@ -1507,7 +1507,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.5482555082611948</v>
+        <v>0.1859502718458239</v>
       </c>
     </row>
     <row r="44">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.5482555082611948</v>
+        <v>0.1859502718458239</v>
       </c>
     </row>
     <row r="45">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.5801065197485813</v>
+        <v>0.2161799568770901</v>
       </c>
     </row>
     <row r="46">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.6432571782636488</v>
+        <v>0.224757668412062</v>
       </c>
     </row>
     <row r="47">
@@ -1607,7 +1607,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.6432571782636488</v>
+        <v>0.224757668412062</v>
       </c>
     </row>
     <row r="48">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.6978123284192081</v>
+        <v>0.2462436466591153</v>
       </c>
     </row>
     <row r="49">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.6329902989806324</v>
+        <v>0.2474733750560441</v>
       </c>
     </row>
     <row r="50">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.6585521390664792</v>
+        <v>0.2482401013263923</v>
       </c>
     </row>
     <row r="51">
@@ -1707,7 +1707,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.6745876979985735</v>
+        <v>0.2464001466138338</v>
       </c>
     </row>
     <row r="52">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>0.6322283007682168</v>
+        <v>0.2172006838600167</v>
       </c>
     </row>
     <row r="53">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0.6322283007682168</v>
+        <v>0.2172006838600167</v>
       </c>
     </row>
     <row r="54">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0.9358487851385324</v>
+        <v>0.2912154967317269</v>
       </c>
     </row>
     <row r="55">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>0.6234123664675494</v>
+        <v>0.2418821162955295</v>
       </c>
     </row>
     <row r="56">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>0.7087085007607341</v>
+        <v>0.2359413849423585</v>
       </c>
     </row>
     <row r="57">
@@ -1848,7 +1848,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>0.7087085007607341</v>
+        <v>0.2359413849423585</v>
       </c>
     </row>
     <row r="58">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>0.5747411420018692</v>
+        <v>0.1918576506515033</v>
       </c>
     </row>
     <row r="59">
@@ -1907,7 +1907,7 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>0.5747411420018692</v>
+        <v>0.1918576506515033</v>
       </c>
     </row>
     <row r="60">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>0.9358487851385324</v>
+        <v>0.2912154967317269</v>
       </c>
     </row>
     <row r="61">
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>0.5715307069637751</v>
+        <v>0.2132581615811058</v>
       </c>
     </row>
     <row r="62">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0.6170353090551565</v>
+        <v>0.2360912561486022</v>
       </c>
     </row>
     <row r="63">
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0.5356815604945677</v>
+        <v>0.1729215534242868</v>
       </c>
     </row>
     <row r="64">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.7986759332836064</v>
+        <v>0.257880451389456</v>
       </c>
     </row>
     <row r="65">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2057,7 +2057,7 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.597235757098174</v>
+        <v>0.2143683180855551</v>
       </c>
     </row>
     <row r="66">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>0.5964032309523206</v>
+        <v>0.2126139642476344</v>
       </c>
     </row>
     <row r="67">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>0.6060989954553004</v>
+        <v>0.2162286050189215</v>
       </c>
     </row>
     <row r="68">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0.5791889880996524</v>
+        <v>0.2133236512507224</v>
       </c>
     </row>
     <row r="69">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2157,7 +2157,7 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0.6059374150246801</v>
+        <v>0.2187879367602779</v>
       </c>
     </row>
     <row r="70">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>0.6151176399470756</v>
+        <v>0.2239797092855502</v>
       </c>
     </row>
     <row r="71">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2207,7 +2207,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.6087674269315593</v>
+        <v>0.2185564365214284</v>
       </c>
     </row>
     <row r="72">
@@ -2223,7 +2223,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.6127265353769945</v>
+        <v>0.2235125960545753</v>
       </c>
     </row>
     <row r="73">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0.6119671581347668</v>
+        <v>0.2179340211334361</v>
       </c>
     </row>
     <row r="74">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.6270374365023051</v>
+        <v>0.2215444716900458</v>
       </c>
     </row>
     <row r="75">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2307,7 +2307,7 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.6051261981345394</v>
+        <v>0.2168362004364179</v>
       </c>
     </row>
     <row r="76">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2332,7 +2332,7 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.6220555031283166</v>
+        <v>0.2192007027486667</v>
       </c>
     </row>
     <row r="77">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2357,7 +2357,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.5748655077705599</v>
+        <v>0.2087408007623403</v>
       </c>
     </row>
     <row r="78">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.594893114402959</v>
+        <v>0.2121255855239745</v>
       </c>
     </row>
     <row r="79">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.6264663850466726</v>
+        <v>0.2042076797975834</v>
       </c>
     </row>
     <row r="80">
@@ -2432,7 +2432,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.5816175872085968</v>
+        <v>0.1807571435627092</v>
       </c>
     </row>
     <row r="81">
@@ -2448,7 +2448,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.5823527245361076</v>
+        <v>0.2099465043138839</v>
       </c>
     </row>
     <row r="82">
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.551248941870538</v>
+        <v>0.1942939590207775</v>
       </c>
     </row>
     <row r="83">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2507,7 +2507,7 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0.5580661006315075</v>
+        <v>0.2006051498303507</v>
       </c>
     </row>
     <row r="84">
@@ -2532,7 +2532,7 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.6087154125497588</v>
+        <v>0.2197491377462429</v>
       </c>
     </row>
     <row r="85">
@@ -2557,7 +2557,7 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.5727211273819642</v>
+        <v>0.1930883051775956</v>
       </c>
     </row>
     <row r="86">
@@ -2582,7 +2582,7 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.6556957718671075</v>
+        <v>0.2162556071697961</v>
       </c>
     </row>
     <row r="87">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2607,7 +2607,7 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.6319536540005015</v>
+        <v>0.2572981448330454</v>
       </c>
     </row>
     <row r="88">
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.6572995506493537</v>
+        <v>0.2197259209933689</v>
       </c>
     </row>
     <row r="89">
@@ -2657,7 +2657,7 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.7029086074781965</v>
+        <v>0.2491538575633987</v>
       </c>
     </row>
     <row r="90">
@@ -2682,7 +2682,7 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>0.689879226583883</v>
+        <v>0.2166992155331422</v>
       </c>
     </row>
     <row r="91">
@@ -2707,7 +2707,7 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0.6125883774244851</v>
+        <v>0.2232725273899429</v>
       </c>
     </row>
     <row r="92">
@@ -2732,7 +2732,7 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0.597476634060498</v>
+        <v>0.2161571074736807</v>
       </c>
     </row>
     <row r="93">
@@ -2748,7 +2748,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2757,7 +2757,7 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0.5565080026278146</v>
+        <v>0.1930251914241153</v>
       </c>
     </row>
     <row r="94">
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>0.6322844014878963</v>
+        <v>0.2008317439423093</v>
       </c>
     </row>
     <row r="95">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0.6119679392167462</v>
+        <v>0.1915771082699911</v>
       </c>
     </row>
     <row r="96">
@@ -2823,7 +2823,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0.6119679392167462</v>
+        <v>0.1915771082699911</v>
       </c>
     </row>
     <row r="97">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2857,7 +2857,7 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.5690871980994012</v>
+        <v>0.1983692288894978</v>
       </c>
     </row>
     <row r="98">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.5480275617912871</v>
+        <v>0.1801423387299256</v>
       </c>
     </row>
     <row r="99">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>0.5480275617912871</v>
+        <v>0.1801423387299256</v>
       </c>
     </row>
     <row r="100">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0.6061852650000823</v>
+        <v>0.1977725069049746</v>
       </c>
     </row>
     <row r="101">
@@ -2957,7 +2957,7 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.5604340409674339</v>
+        <v>0.193136133340538</v>
       </c>
     </row>
     <row r="102">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0.624652884339721</v>
+        <v>0.2021967701219878</v>
       </c>
     </row>
     <row r="103">
@@ -2998,7 +2998,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3007,7 +3007,7 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.6566125001295722</v>
+        <v>0.236185075747</v>
       </c>
     </row>
     <row r="104">
@@ -3032,7 +3032,7 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>0.5970461132102471</v>
+        <v>0.2176904113152706</v>
       </c>
     </row>
     <row r="105">
@@ -3048,7 +3048,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0.6516624911253037</v>
+        <v>0.2312099543650209</v>
       </c>
     </row>
     <row r="106">
@@ -3073,7 +3073,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3082,7 +3082,7 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0.5863605913440439</v>
+        <v>0.2162956241550933</v>
       </c>
     </row>
     <row r="107">
@@ -3107,7 +3107,7 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0.6592956475472946</v>
+        <v>0.2365807909164496</v>
       </c>
     </row>
     <row r="108">
@@ -3132,7 +3132,7 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0.6140413386708432</v>
+        <v>0.2048462773282919</v>
       </c>
     </row>
     <row r="109">
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="E109" t="n">
-        <v>0.5739420686362774</v>
+        <v>0.1995072071323092</v>
       </c>
     </row>
     <row r="110">
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.5608710647541718</v>
+        <v>0.1909307740449807</v>
       </c>
     </row>
     <row r="111">
@@ -3207,7 +3207,7 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>0.5436471162267201</v>
+        <v>0.1791252610405064</v>
       </c>
     </row>
     <row r="112">
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0.5348007685608206</v>
+        <v>0.1841692948101548</v>
       </c>
     </row>
     <row r="113">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3257,7 +3257,7 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>0.700280118984405</v>
+        <v>0.2031039714917229</v>
       </c>
     </row>
     <row r="114">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0.6785881617830791</v>
+        <v>0.2411696432842189</v>
       </c>
     </row>
     <row r="115">
@@ -3307,7 +3307,7 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>0.564725189110267</v>
+        <v>0.1832100649193996</v>
       </c>
     </row>
     <row r="116">
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>0.6680321817957792</v>
+        <v>0.2390467500323848</v>
       </c>
     </row>
     <row r="117">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3357,7 +3357,7 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>0.5968168776128713</v>
+        <v>0.2127961293779178</v>
       </c>
     </row>
     <row r="118">
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="E118" t="n">
-        <v>0.6875826849091763</v>
+        <v>0.2441993444123325</v>
       </c>
     </row>
     <row r="119">
@@ -3407,7 +3407,7 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>0.5718188556908411</v>
+        <v>0.1977569806676631</v>
       </c>
     </row>
     <row r="120">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>0.5765003361170051</v>
+        <v>0.2070585236932813</v>
       </c>
     </row>
     <row r="121">
@@ -3457,7 +3457,7 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0.6655729291793567</v>
+        <v>0.2426789816816356</v>
       </c>
     </row>
     <row r="122">
@@ -3482,7 +3482,7 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>0.6440185248159238</v>
+        <v>0.2065915333986136</v>
       </c>
     </row>
     <row r="123">
@@ -3507,7 +3507,7 @@
         </is>
       </c>
       <c r="E123" t="n">
-        <v>0.611008019129605</v>
+        <v>0.2123564544832353</v>
       </c>
     </row>
     <row r="124">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3532,7 +3532,7 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>0.6531417355401377</v>
+        <v>0.2195193104447803</v>
       </c>
     </row>
     <row r="125">
@@ -3548,7 +3548,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3557,7 +3557,7 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>0.6815444013742791</v>
+        <v>0.2318554446232464</v>
       </c>
     </row>
     <row r="126">
@@ -3582,7 +3582,7 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>0.5380813790410808</v>
+        <v>0.1718334556657107</v>
       </c>
     </row>
     <row r="127">
@@ -3607,7 +3607,7 @@
         </is>
       </c>
       <c r="E127" t="n">
-        <v>0.5380813790410808</v>
+        <v>0.1718334556657107</v>
       </c>
     </row>
     <row r="128">
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>0.6140953522673924</v>
+        <v>0.2138347978241541</v>
       </c>
     </row>
     <row r="129">
@@ -3657,7 +3657,7 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>0.5112098359215059</v>
+        <v>0.1762182114671484</v>
       </c>
     </row>
     <row r="130">
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>0.5112098359215059</v>
+        <v>0.1762182114671484</v>
       </c>
     </row>
     <row r="131">
@@ -3698,7 +3698,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3707,7 +3707,7 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>0.6834763384752626</v>
+        <v>0.2201242701216267</v>
       </c>
     </row>
     <row r="132">
@@ -3732,7 +3732,7 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>0.5983606742565071</v>
+        <v>0.2326788127931043</v>
       </c>
     </row>
     <row r="133">
@@ -3757,7 +3757,7 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0.5641521719581547</v>
+        <v>0.1958988579539944</v>
       </c>
     </row>
     <row r="134">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3782,7 +3782,7 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>0.6667799992654636</v>
+        <v>0.1990633777644832</v>
       </c>
     </row>
     <row r="135">
@@ -3807,7 +3807,7 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>0.5535057927953562</v>
+        <v>0.1814454682524877</v>
       </c>
     </row>
     <row r="136">
@@ -3823,7 +3823,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>0.6518979169676727</v>
+        <v>0.2329480103359224</v>
       </c>
     </row>
     <row r="137">
@@ -3857,7 +3857,7 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0.635621659059296</v>
+        <v>0.2337981401633577</v>
       </c>
     </row>
     <row r="138">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>0.6256987649815517</v>
+        <v>0.2116546391659941</v>
       </c>
     </row>
     <row r="139">
@@ -3907,7 +3907,7 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>0.6920849243147192</v>
+        <v>0.2436634220228177</v>
       </c>
     </row>
     <row r="140">
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>0.6846680397160806</v>
+        <v>0.2408071374759375</v>
       </c>
     </row>
     <row r="141">
@@ -3957,7 +3957,7 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>0.5552099578490749</v>
+        <v>0.1894993475171643</v>
       </c>
     </row>
     <row r="142">
@@ -3982,7 +3982,7 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>0.6867315481381757</v>
+        <v>0.2184211862198918</v>
       </c>
     </row>
     <row r="143">
@@ -4007,7 +4007,7 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>0.6226865768363923</v>
+        <v>0.2091782824553058</v>
       </c>
     </row>
     <row r="144">
@@ -4032,7 +4032,7 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>0.69185212743886</v>
+        <v>0.2466008072818586</v>
       </c>
     </row>
     <row r="145">
@@ -4057,7 +4057,7 @@
         </is>
       </c>
       <c r="E145" t="n">
-        <v>0.6240995391217045</v>
+        <v>0.1989119239799816</v>
       </c>
     </row>
     <row r="146">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4082,7 +4082,7 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>0.6986081461222095</v>
+        <v>0.2271769639913267</v>
       </c>
     </row>
     <row r="147">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4107,7 +4107,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>0.5410678206768812</v>
+        <v>0.1817814691374956</v>
       </c>
     </row>
     <row r="148">
@@ -4132,7 +4132,7 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>0.6949363833754211</v>
+        <v>0.2470349261240072</v>
       </c>
     </row>
     <row r="149">
@@ -4157,7 +4157,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>0.6659942269888279</v>
+        <v>0.2441060387171928</v>
       </c>
     </row>
     <row r="150">
@@ -4182,7 +4182,7 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>0.5874716331368065</v>
+        <v>0.2090065244320926</v>
       </c>
     </row>
     <row r="151">
@@ -4207,7 +4207,7 @@
         </is>
       </c>
       <c r="E151" t="n">
-        <v>0.5691297004314083</v>
+        <v>0.1930981692612968</v>
       </c>
     </row>
     <row r="152">
@@ -4232,7 +4232,7 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>0.5614261451120807</v>
+        <v>0.1944617342355039</v>
       </c>
     </row>
     <row r="153">
@@ -4257,7 +4257,7 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>0.6877940862410374</v>
+        <v>0.2439058333272131</v>
       </c>
     </row>
     <row r="154">
@@ -4282,7 +4282,7 @@
         </is>
       </c>
       <c r="E154" t="n">
-        <v>0.7256233824375428</v>
+        <v>0.2194328640631647</v>
       </c>
     </row>
     <row r="155">
@@ -4307,7 +4307,7 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>0.6974494533209993</v>
+        <v>0.2451620108094628</v>
       </c>
     </row>
     <row r="156">
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="E156" t="n">
-        <v>0.661961116924917</v>
+        <v>0.2465879814848008</v>
       </c>
     </row>
     <row r="157">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4357,7 +4357,7 @@
         </is>
       </c>
       <c r="E157" t="n">
-        <v>0.6624516652843875</v>
+        <v>0.2240872335783986</v>
       </c>
     </row>
     <row r="158">
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="E158" t="n">
-        <v>0.6785698938873888</v>
+        <v>0.2465318223307043</v>
       </c>
     </row>
     <row r="159">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>0.6259649146653629</v>
+        <v>0.2025431120136024</v>
       </c>
     </row>
     <row r="160">
@@ -4432,7 +4432,7 @@
         </is>
       </c>
       <c r="E160" t="n">
-        <v>0.6259649146653629</v>
+        <v>0.2025431120136024</v>
       </c>
     </row>
     <row r="161">
@@ -4457,7 +4457,7 @@
         </is>
       </c>
       <c r="E161" t="n">
-        <v>0.5721511569601969</v>
+        <v>0.2054718230163724</v>
       </c>
     </row>
     <row r="162">
@@ -4482,7 +4482,7 @@
         </is>
       </c>
       <c r="E162" t="n">
-        <v>0.5995935717750793</v>
+        <v>0.1884091213601555</v>
       </c>
     </row>
     <row r="163">
@@ -4507,7 +4507,7 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>0.5995935717750793</v>
+        <v>0.1884091213601555</v>
       </c>
     </row>
     <row r="164">
@@ -4532,7 +4532,7 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>0.6669702411682537</v>
+        <v>0.2414006405185085</v>
       </c>
     </row>
     <row r="165">
@@ -4557,7 +4557,7 @@
         </is>
       </c>
       <c r="E165" t="n">
-        <v>0.5677108792699662</v>
+        <v>0.2003240931492496</v>
       </c>
     </row>
     <row r="166">
@@ -4582,7 +4582,7 @@
         </is>
       </c>
       <c r="E166" t="n">
-        <v>0.5241378768734777</v>
+        <v>0.1749353311167443</v>
       </c>
     </row>
     <row r="167">
@@ -4607,7 +4607,7 @@
         </is>
       </c>
       <c r="E167" t="n">
-        <v>0.6383701097624043</v>
+        <v>0.2006471271890234</v>
       </c>
     </row>
     <row r="168">
@@ -4632,7 +4632,7 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>0.6383701097624043</v>
+        <v>0.2006471271890234</v>
       </c>
     </row>
     <row r="169">
@@ -4648,7 +4648,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -4657,7 +4657,7 @@
         </is>
       </c>
       <c r="E169" t="n">
-        <v>0.6309033470802077</v>
+        <v>0.2106803469448182</v>
       </c>
     </row>
     <row r="170">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -4682,7 +4682,7 @@
         </is>
       </c>
       <c r="E170" t="n">
-        <v>0.6076973419552618</v>
+        <v>0.184318179199296</v>
       </c>
     </row>
     <row r="171">
@@ -4698,7 +4698,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -4707,7 +4707,7 @@
         </is>
       </c>
       <c r="E171" t="n">
-        <v>0.6076973419552618</v>
+        <v>0.184318179199296</v>
       </c>
     </row>
     <row r="172">
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="E172" t="n">
-        <v>0.5270145249463208</v>
+        <v>0.1817371325710435</v>
       </c>
     </row>
     <row r="173">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -4757,7 +4757,7 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>0.5734978358499141</v>
+        <v>0.2031616199686088</v>
       </c>
     </row>
     <row r="174">
@@ -4782,7 +4782,7 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>0.6621156754957132</v>
+        <v>0.2411783640540222</v>
       </c>
     </row>
     <row r="175">
@@ -4807,7 +4807,7 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>0.554942403725266</v>
+        <v>0.1951345133361378</v>
       </c>
     </row>
     <row r="176">
@@ -4832,7 +4832,7 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>0.5592027951547028</v>
+        <v>0.1874872324182414</v>
       </c>
     </row>
     <row r="177">
@@ -4857,7 +4857,7 @@
         </is>
       </c>
       <c r="E177" t="n">
-        <v>0.607945166038486</v>
+        <v>0.2149965489529136</v>
       </c>
     </row>
     <row r="178">
@@ -4882,7 +4882,7 @@
         </is>
       </c>
       <c r="E178" t="n">
-        <v>0.5937733610457864</v>
+        <v>0.2014044198075386</v>
       </c>
     </row>
     <row r="179">
@@ -4907,7 +4907,7 @@
         </is>
       </c>
       <c r="E179" t="n">
-        <v>0.6771617322791955</v>
+        <v>0.2463448379919782</v>
       </c>
     </row>
     <row r="180">
@@ -4923,7 +4923,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="E180" t="n">
-        <v>0.7078015338689345</v>
+        <v>0.2111638473786103</v>
       </c>
     </row>
     <row r="181">
@@ -4957,7 +4957,7 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>0.5216574726305414</v>
+        <v>0.165702739283337</v>
       </c>
     </row>
     <row r="182">
@@ -4973,7 +4973,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -4982,7 +4982,7 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>0.5794746523012284</v>
+        <v>0.2178547476705149</v>
       </c>
     </row>
     <row r="183">
@@ -5007,7 +5007,7 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>0.642457558957568</v>
+        <v>0.230365753058148</v>
       </c>
     </row>
     <row r="184">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -5032,7 +5032,7 @@
         </is>
       </c>
       <c r="E184" t="n">
-        <v>0.5539725708379299</v>
+        <v>0.1847941202957803</v>
       </c>
     </row>
     <row r="185">
@@ -5057,7 +5057,7 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>0.6701871658169177</v>
+        <v>0.2432506767308327</v>
       </c>
     </row>
     <row r="186">
@@ -5082,7 +5082,7 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>0.6334425984224913</v>
+        <v>0.2137897467865802</v>
       </c>
     </row>
     <row r="187">
@@ -5107,7 +5107,7 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>0.5597900669444522</v>
+        <v>0.2036271155082193</v>
       </c>
     </row>
     <row r="188">
@@ -5123,7 +5123,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -5132,7 +5132,7 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>0.6310394144832252</v>
+        <v>0.2151060067839535</v>
       </c>
     </row>
     <row r="189">
@@ -5157,7 +5157,7 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>0.6161757963989567</v>
+        <v>0.1959748763835022</v>
       </c>
     </row>
     <row r="190">
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>0.6146393861418078</v>
+        <v>0.2122450856888591</v>
       </c>
     </row>
     <row r="191">
@@ -5207,7 +5207,7 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>0.6445522180914691</v>
+        <v>0.2164823001355428</v>
       </c>
     </row>
     <row r="192">
@@ -5232,7 +5232,7 @@
         </is>
       </c>
       <c r="E192" t="n">
-        <v>0.6036984964065735</v>
+        <v>0.2103437498954052</v>
       </c>
     </row>
     <row r="193">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -5257,7 +5257,7 @@
         </is>
       </c>
       <c r="E193" t="n">
-        <v>0.5746634808833193</v>
+        <v>0.1901563692260312</v>
       </c>
     </row>
     <row r="194">
@@ -5282,7 +5282,7 @@
         </is>
       </c>
       <c r="E194" t="n">
-        <v>0.5748408012544199</v>
+        <v>0.1810163472120782</v>
       </c>
     </row>
     <row r="195">
@@ -5307,7 +5307,7 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>0.6266164948005364</v>
+        <v>0.2114340620386445</v>
       </c>
     </row>
     <row r="196">
@@ -5332,7 +5332,7 @@
         </is>
       </c>
       <c r="E196" t="n">
-        <v>0.5810814370973297</v>
+        <v>0.2067235587403751</v>
       </c>
     </row>
     <row r="197">
@@ -5357,7 +5357,7 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>0.5443894728242649</v>
+        <v>0.194318859387294</v>
       </c>
     </row>
     <row r="198">
@@ -5373,7 +5373,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -5382,7 +5382,7 @@
         </is>
       </c>
       <c r="E198" t="n">
-        <v>0.559039517750948</v>
+        <v>0.1875075693627212</v>
       </c>
     </row>
     <row r="199">
@@ -5407,7 +5407,7 @@
         </is>
       </c>
       <c r="E199" t="n">
-        <v>0.5770990507687996</v>
+        <v>0.1918264415797476</v>
       </c>
     </row>
     <row r="200">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -5432,7 +5432,7 @@
         </is>
       </c>
       <c r="E200" t="n">
-        <v>0.9358487851385324</v>
+        <v>0.2912154967317269</v>
       </c>
     </row>
     <row r="201">
@@ -5448,7 +5448,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -5457,7 +5457,7 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>0.5710160620501934</v>
+        <v>0.1805584933339006</v>
       </c>
     </row>
     <row r="202">
@@ -5482,7 +5482,7 @@
         </is>
       </c>
       <c r="E202" t="n">
-        <v>0.5583307268748228</v>
+        <v>0.1774146601083935</v>
       </c>
     </row>
     <row r="203">
@@ -5507,7 +5507,7 @@
         </is>
       </c>
       <c r="E203" t="n">
-        <v>0.5770352214192708</v>
+        <v>0.2005130767672227</v>
       </c>
     </row>
     <row r="204">
@@ -5532,7 +5532,7 @@
         </is>
       </c>
       <c r="E204" t="n">
-        <v>0.6251142381267812</v>
+        <v>0.2070809493703263</v>
       </c>
     </row>
     <row r="205">
@@ -5548,7 +5548,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -5557,7 +5557,7 @@
         </is>
       </c>
       <c r="E205" t="n">
-        <v>0.5841545745031483</v>
+        <v>0.2165452013425795</v>
       </c>
     </row>
     <row r="206">
@@ -5582,7 +5582,7 @@
         </is>
       </c>
       <c r="E206" t="n">
-        <v>0.5688775006711722</v>
+        <v>0.1941887854218077</v>
       </c>
     </row>
     <row r="207">
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>0.5855641405299689</v>
+        <v>0.2021162614236721</v>
       </c>
     </row>
     <row r="208">
@@ -5632,7 +5632,7 @@
         </is>
       </c>
       <c r="E208" t="n">
-        <v>0.5233025131447935</v>
+        <v>0.1738546107437495</v>
       </c>
     </row>
     <row r="209">
@@ -5657,7 +5657,7 @@
         </is>
       </c>
       <c r="E209" t="n">
-        <v>0.577784883295081</v>
+        <v>0.1964089147882169</v>
       </c>
     </row>
     <row r="210">
@@ -5673,7 +5673,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -5682,7 +5682,7 @@
         </is>
       </c>
       <c r="E210" t="n">
-        <v>0.5325654548522286</v>
+        <v>0.174927438542869</v>
       </c>
     </row>
     <row r="211">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -5707,7 +5707,7 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>0.5793256643627384</v>
+        <v>0.1978565795283808</v>
       </c>
     </row>
     <row r="212">
@@ -5723,7 +5723,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -5732,7 +5732,7 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>0.6641615784456034</v>
+        <v>0.2078519715706385</v>
       </c>
     </row>
     <row r="213">
@@ -5757,7 +5757,7 @@
         </is>
       </c>
       <c r="E213" t="n">
-        <v>0.6132520150076257</v>
+        <v>0.2403973213312887</v>
       </c>
     </row>
     <row r="214">
@@ -5782,7 +5782,7 @@
         </is>
       </c>
       <c r="E214" t="n">
-        <v>0.6513987567114548</v>
+        <v>0.2482811026262685</v>
       </c>
     </row>
     <row r="215">
@@ -5807,7 +5807,7 @@
         </is>
       </c>
       <c r="E215" t="n">
-        <v>0.547854436641007</v>
+        <v>0.1853153812698123</v>
       </c>
     </row>
     <row r="216">
@@ -5832,7 +5832,7 @@
         </is>
       </c>
       <c r="E216" t="n">
-        <v>0.5380917324810757</v>
+        <v>0.1805304795338828</v>
       </c>
     </row>
     <row r="217">
@@ -5857,7 +5857,7 @@
         </is>
       </c>
       <c r="E217" t="n">
-        <v>0.5389094267467388</v>
+        <v>0.1845009828703107</v>
       </c>
     </row>
     <row r="218">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
@@ -5882,7 +5882,7 @@
         </is>
       </c>
       <c r="E218" t="n">
-        <v>0.5742454196625142</v>
+        <v>0.1947699462469984</v>
       </c>
     </row>
     <row r="219">
@@ -5907,7 +5907,7 @@
         </is>
       </c>
       <c r="E219" t="n">
-        <v>0.5388348090803166</v>
+        <v>0.18354643262743</v>
       </c>
     </row>
     <row r="220">
@@ -5932,7 +5932,7 @@
         </is>
       </c>
       <c r="E220" t="n">
-        <v>0.5350923071923616</v>
+        <v>0.1743209481481302</v>
       </c>
     </row>
     <row r="221">
@@ -5948,7 +5948,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -5957,7 +5957,7 @@
         </is>
       </c>
       <c r="E221" t="n">
-        <v>0.5647052630152586</v>
+        <v>0.1995318093141773</v>
       </c>
     </row>
     <row r="222">
@@ -5973,7 +5973,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -5982,7 +5982,7 @@
         </is>
       </c>
       <c r="E222" t="n">
-        <v>0.6368511130016821</v>
+        <v>0.2181035255585674</v>
       </c>
     </row>
     <row r="223">
@@ -6007,7 +6007,7 @@
         </is>
       </c>
       <c r="E223" t="n">
-        <v>0.6566415248509826</v>
+        <v>0.2197733996509396</v>
       </c>
     </row>
     <row r="224">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -6032,7 +6032,7 @@
         </is>
       </c>
       <c r="E224" t="n">
-        <v>0.5462867045541294</v>
+        <v>0.1846468980739309</v>
       </c>
     </row>
     <row r="225">
@@ -6048,7 +6048,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -6057,7 +6057,7 @@
         </is>
       </c>
       <c r="E225" t="n">
-        <v>0.9358487851385324</v>
+        <v>0.2912154967317269</v>
       </c>
     </row>
     <row r="226">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -6082,7 +6082,7 @@
         </is>
       </c>
       <c r="E226" t="n">
-        <v>0.6267922790005784</v>
+        <v>0.2474001575781601</v>
       </c>
     </row>
     <row r="227">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -6107,7 +6107,7 @@
         </is>
       </c>
       <c r="E227" t="n">
-        <v>0.6474820811225568</v>
+        <v>0.1951176488733339</v>
       </c>
     </row>
     <row r="228">
@@ -6132,7 +6132,7 @@
         </is>
       </c>
       <c r="E228" t="n">
-        <v>0.5522132026825672</v>
+        <v>0.192253003887892</v>
       </c>
     </row>
     <row r="229">
@@ -6157,7 +6157,7 @@
         </is>
       </c>
       <c r="E229" t="n">
-        <v>0.6785378054510637</v>
+        <v>0.2174452062699976</v>
       </c>
     </row>
     <row r="230">
@@ -6173,7 +6173,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -6182,7 +6182,7 @@
         </is>
       </c>
       <c r="E230" t="n">
-        <v>0.5933854251051743</v>
+        <v>0.21494008255421</v>
       </c>
     </row>
     <row r="231">
@@ -6198,7 +6198,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -6207,7 +6207,7 @@
         </is>
       </c>
       <c r="E231" t="n">
-        <v>0.6204727299032645</v>
+        <v>0.2187195941522005</v>
       </c>
     </row>
     <row r="232">
@@ -6232,7 +6232,7 @@
         </is>
       </c>
       <c r="E232" t="n">
-        <v>0.5997004773698306</v>
+        <v>0.2038770335909658</v>
       </c>
     </row>
     <row r="233">
@@ -6257,7 +6257,7 @@
         </is>
       </c>
       <c r="E233" t="n">
-        <v>0.6661827738080265</v>
+        <v>0.2419898902719332</v>
       </c>
     </row>
     <row r="234">
@@ -6282,7 +6282,7 @@
         </is>
       </c>
       <c r="E234" t="n">
-        <v>0.6101134508128595</v>
+        <v>0.2378656303738035</v>
       </c>
     </row>
     <row r="235">
@@ -6307,7 +6307,7 @@
         </is>
       </c>
       <c r="E235" t="n">
-        <v>0.6861804956359876</v>
+        <v>0.2442293436300115</v>
       </c>
     </row>
     <row r="236">
@@ -6332,7 +6332,7 @@
         </is>
       </c>
       <c r="E236" t="n">
-        <v>0.5879722310427935</v>
+        <v>0.1931564222390507</v>
       </c>
     </row>
     <row r="237">
@@ -6348,7 +6348,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -6357,7 +6357,7 @@
         </is>
       </c>
       <c r="E237" t="n">
-        <v>0.6043665178094468</v>
+        <v>0.219218417819668</v>
       </c>
     </row>
     <row r="238">
@@ -6373,7 +6373,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -6382,7 +6382,7 @@
         </is>
       </c>
       <c r="E238" t="n">
-        <v>0.5969820802481407</v>
+        <v>0.2151562893238727</v>
       </c>
     </row>
     <row r="239">
@@ -6407,7 +6407,7 @@
         </is>
       </c>
       <c r="E239" t="n">
-        <v>0.5813509517738992</v>
+        <v>0.2095455286850894</v>
       </c>
     </row>
     <row r="240">
@@ -6432,7 +6432,7 @@
         </is>
       </c>
       <c r="E240" t="n">
-        <v>0.6136827605321441</v>
+        <v>0.2404301176682897</v>
       </c>
     </row>
     <row r="241">
@@ -6448,7 +6448,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -6457,7 +6457,7 @@
         </is>
       </c>
       <c r="E241" t="n">
-        <v>0.56921448429402</v>
+        <v>0.2098558949548522</v>
       </c>
     </row>
     <row r="242">
@@ -6473,7 +6473,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -6482,7 +6482,7 @@
         </is>
       </c>
       <c r="E242" t="n">
-        <v>0.5921758284428809</v>
+        <v>0.213207021848421</v>
       </c>
     </row>
     <row r="243">
@@ -6498,7 +6498,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -6507,7 +6507,7 @@
         </is>
       </c>
       <c r="E243" t="n">
-        <v>0.5857862110786869</v>
+        <v>0.2153911527706773</v>
       </c>
     </row>
     <row r="244">
@@ -6523,7 +6523,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -6532,7 +6532,7 @@
         </is>
       </c>
       <c r="E244" t="n">
-        <v>0.6075669005618194</v>
+        <v>0.217134234859881</v>
       </c>
     </row>
     <row r="245">
@@ -6548,7 +6548,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -6557,7 +6557,7 @@
         </is>
       </c>
       <c r="E245" t="n">
-        <v>0.6393556942818596</v>
+        <v>0.2164126614700176</v>
       </c>
     </row>
     <row r="246">
@@ -6573,7 +6573,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -6582,7 +6582,7 @@
         </is>
       </c>
       <c r="E246" t="n">
-        <v>0.5817034717122137</v>
+        <v>0.2118934043473161</v>
       </c>
     </row>
     <row r="247">
@@ -6598,7 +6598,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -6607,7 +6607,7 @@
         </is>
       </c>
       <c r="E247" t="n">
-        <v>0.5904638365011333</v>
+        <v>0.2169366289424186</v>
       </c>
     </row>
     <row r="248">
@@ -6632,7 +6632,7 @@
         </is>
       </c>
       <c r="E248" t="n">
-        <v>0.6038943362405437</v>
+        <v>0.2164112127533795</v>
       </c>
     </row>
     <row r="249">
@@ -6648,7 +6648,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -6657,7 +6657,7 @@
         </is>
       </c>
       <c r="E249" t="n">
-        <v>0.628037282631169</v>
+        <v>0.221733850145002</v>
       </c>
     </row>
     <row r="250">
@@ -6673,7 +6673,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -6682,7 +6682,7 @@
         </is>
       </c>
       <c r="E250" t="n">
-        <v>0.5678673487973519</v>
+        <v>0.2119960834052574</v>
       </c>
     </row>
     <row r="251">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -6707,7 +6707,7 @@
         </is>
       </c>
       <c r="E251" t="n">
-        <v>0.6010518900447294</v>
+        <v>0.2209809616853964</v>
       </c>
     </row>
     <row r="252">
@@ -6723,7 +6723,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
@@ -6732,7 +6732,7 @@
         </is>
       </c>
       <c r="E252" t="n">
-        <v>0.6189718390676795</v>
+        <v>0.221000734602897</v>
       </c>
     </row>
     <row r="253">
@@ -6748,7 +6748,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -6757,7 +6757,7 @@
         </is>
       </c>
       <c r="E253" t="n">
-        <v>0.5596534556462073</v>
+        <v>0.2093162271235336</v>
       </c>
     </row>
     <row r="254">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -6782,7 +6782,7 @@
         </is>
       </c>
       <c r="E254" t="n">
-        <v>0.5712952500036077</v>
+        <v>0.2088770064172286</v>
       </c>
     </row>
     <row r="255">
@@ -6798,7 +6798,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -6807,7 +6807,7 @@
         </is>
       </c>
       <c r="E255" t="n">
-        <v>0.5699368914299614</v>
+        <v>0.1917578015457137</v>
       </c>
     </row>
     <row r="256">
@@ -6823,7 +6823,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -6832,7 +6832,7 @@
         </is>
       </c>
       <c r="E256" t="n">
-        <v>0.5924359556671361</v>
+        <v>0.2040016879389153</v>
       </c>
     </row>
     <row r="257">
@@ -6857,7 +6857,7 @@
         </is>
       </c>
       <c r="E257" t="n">
-        <v>0.6144652813691834</v>
+        <v>0.2291728881300586</v>
       </c>
     </row>
     <row r="258">
@@ -6882,7 +6882,7 @@
         </is>
       </c>
       <c r="E258" t="n">
-        <v>0.6349235551838359</v>
+        <v>0.220322077069066</v>
       </c>
     </row>
     <row r="259">
@@ -6898,7 +6898,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -6907,7 +6907,7 @@
         </is>
       </c>
       <c r="E259" t="n">
-        <v>0.6804110631464884</v>
+        <v>0.2262813400634003</v>
       </c>
     </row>
     <row r="260">
@@ -6932,7 +6932,7 @@
         </is>
       </c>
       <c r="E260" t="n">
-        <v>0.5603430491504079</v>
+        <v>0.1920661857330521</v>
       </c>
     </row>
     <row r="261">
@@ -6957,7 +6957,7 @@
         </is>
       </c>
       <c r="E261" t="n">
-        <v>0.5279827299364113</v>
+        <v>0.1781030956726832</v>
       </c>
     </row>
     <row r="262">
@@ -6982,7 +6982,7 @@
         </is>
       </c>
       <c r="E262" t="n">
-        <v>0.5087169359043189</v>
+        <v>0.1692752725519704</v>
       </c>
     </row>
     <row r="263">
@@ -6998,7 +6998,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
@@ -7007,7 +7007,7 @@
         </is>
       </c>
       <c r="E263" t="n">
-        <v>0.5577245603418873</v>
+        <v>0.18611744713539</v>
       </c>
     </row>
     <row r="264">
@@ -7032,7 +7032,7 @@
         </is>
       </c>
       <c r="E264" t="n">
-        <v>0.6216111013995571</v>
+        <v>0.2298375446378776</v>
       </c>
     </row>
     <row r="265">
@@ -7057,7 +7057,7 @@
         </is>
       </c>
       <c r="E265" t="n">
-        <v>0.5488391617122015</v>
+        <v>0.188948893299029</v>
       </c>
     </row>
     <row r="266">
@@ -7073,7 +7073,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
@@ -7082,7 +7082,7 @@
         </is>
       </c>
       <c r="E266" t="n">
-        <v>0.5661465139973576</v>
+        <v>0.1850022765471871</v>
       </c>
     </row>
     <row r="267">
@@ -7107,7 +7107,7 @@
         </is>
       </c>
       <c r="E267" t="n">
-        <v>0.7844327837705544</v>
+        <v>0.2563578335396484</v>
       </c>
     </row>
     <row r="268">
@@ -7123,7 +7123,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>LR3_other</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
@@ -7132,7 +7132,7 @@
         </is>
       </c>
       <c r="E268" t="n">
-        <v>0.6195724569676226</v>
+        <v>0.2397016424370005</v>
       </c>
     </row>
     <row r="269">
@@ -7157,7 +7157,7 @@
         </is>
       </c>
       <c r="E269" t="n">
-        <v>0.6611246329247925</v>
+        <v>0.242406250124769</v>
       </c>
     </row>
     <row r="270">
@@ -7182,7 +7182,7 @@
         </is>
       </c>
       <c r="E270" t="n">
-        <v>0.5653149861533266</v>
+        <v>0.1901796125586574</v>
       </c>
     </row>
     <row r="271">
@@ -7207,7 +7207,7 @@
         </is>
       </c>
       <c r="E271" t="n">
-        <v>0.6022533019489194</v>
+        <v>0.2461113437795834</v>
       </c>
     </row>
     <row r="272">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -7232,7 +7232,7 @@
         </is>
       </c>
       <c r="E272" t="n">
-        <v>0.5713468238213333</v>
+        <v>0.1990431571635409</v>
       </c>
     </row>
     <row r="273">
@@ -7257,7 +7257,7 @@
         </is>
       </c>
       <c r="E273" t="n">
-        <v>0.5314972446574626</v>
+        <v>0.1820537253632367</v>
       </c>
     </row>
     <row r="274">
@@ -7282,7 +7282,7 @@
         </is>
       </c>
       <c r="E274" t="n">
-        <v>0.6385488566807522</v>
+        <v>0.2293500627478006</v>
       </c>
     </row>
     <row r="275">
@@ -7298,7 +7298,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -7307,7 +7307,7 @@
         </is>
       </c>
       <c r="E275" t="n">
-        <v>0.5944196633279932</v>
+        <v>0.2162775417607087</v>
       </c>
     </row>
     <row r="276">
@@ -7323,7 +7323,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
@@ -7332,7 +7332,7 @@
         </is>
       </c>
       <c r="E276" t="n">
-        <v>0.5907198892840466</v>
+        <v>0.1953050041897226</v>
       </c>
     </row>
     <row r="277">
@@ -7357,7 +7357,7 @@
         </is>
       </c>
       <c r="E277" t="n">
-        <v>0.5290770597825606</v>
+        <v>0.1836140055067624</v>
       </c>
     </row>
     <row r="278">
@@ -7382,7 +7382,7 @@
         </is>
       </c>
       <c r="E278" t="n">
-        <v>0.5381146663031597</v>
+        <v>0.1811980331157299</v>
       </c>
     </row>
     <row r="279">
@@ -7407,7 +7407,7 @@
         </is>
       </c>
       <c r="E279" t="n">
-        <v>0.5877928076889798</v>
+        <v>0.2006030994513313</v>
       </c>
     </row>
     <row r="280">
@@ -7423,7 +7423,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR3_other</t>
         </is>
       </c>
       <c r="D280" t="inlineStr">
@@ -7432,7 +7432,7 @@
         </is>
       </c>
       <c r="E280" t="n">
-        <v>0.6416177573049368</v>
+        <v>0.2431494439098693</v>
       </c>
     </row>
     <row r="281">
@@ -7448,7 +7448,7 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>LR2_payload</t>
+          <t>LR1_signalling</t>
         </is>
       </c>
       <c r="D281" t="inlineStr">
@@ -7457,7 +7457,7 @@
         </is>
       </c>
       <c r="E281" t="n">
-        <v>0.5992434250571671</v>
+        <v>0.2050794491632351</v>
       </c>
     </row>
     <row r="282">
@@ -7482,7 +7482,7 @@
         </is>
       </c>
       <c r="E282" t="n">
-        <v>0.6730841288644516</v>
+        <v>0.2136869097740994</v>
       </c>
     </row>
     <row r="283">
@@ -7507,7 +7507,7 @@
         </is>
       </c>
       <c r="E283" t="n">
-        <v>0.5997263297657786</v>
+        <v>0.2277774747163299</v>
       </c>
     </row>
     <row r="284">
@@ -7532,7 +7532,7 @@
         </is>
       </c>
       <c r="E284" t="n">
-        <v>0.568098091905895</v>
+        <v>0.191897677160382</v>
       </c>
     </row>
     <row r="285">
@@ -7548,7 +7548,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>LR1_signalling</t>
+          <t>LR2_payload</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
@@ -7557,7 +7557,7 @@
         </is>
       </c>
       <c r="E285" t="n">
-        <v>0.6717334752078541</v>
+        <v>0.2352269577623529</v>
       </c>
     </row>
     <row r="286">
@@ -7582,7 +7582,7 @@
         </is>
       </c>
       <c r="E286" t="n">
-        <v>0.6259237087152083</v>
+        <v>0.2479561464456308</v>
       </c>
     </row>
     <row r="287">
@@ -7607,7 +7607,7 @@
         </is>
       </c>
       <c r="E287" t="n">
-        <v>0.6165336009229203</v>
+        <v>0.1959133731488898</v>
       </c>
     </row>
     <row r="288">
@@ -7632,7 +7632,7 @@
         </is>
       </c>
       <c r="E288" t="n">
-        <v>0.5423863312815039</v>
+        <v>0.1883268694570163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>